<commit_message>
등호 math_table.xlsx 에 추가
</commit_message>
<xml_diff>
--- a/math_table.xlsx
+++ b/math_table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20356"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daehan_kim\Desktop\hyperstudy\eq2script\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\docker_data\math2kor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F218441-029F-41EC-8E8B-DCA08FA870E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{454C84F3-9034-4D35-A92D-869F6878521D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="123">
   <si>
     <t>a</t>
   </si>
@@ -392,6 +392,14 @@
   </si>
   <si>
     <t>{c}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>=</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>는</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -760,10 +768,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B77"/>
+  <dimension ref="A1:B78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -790,482 +798,482 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>120</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>117</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B18" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B19" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B20" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B21" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B22" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B23" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B25" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B26" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B27" t="s">
-        <v>51</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B28" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B29" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B30" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B31" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B32" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B33" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B34" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B35" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B36" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B37" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B38" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B39" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B40" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B41" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B42" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B43" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B44" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B45" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B46" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B47" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B48" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B49" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B50" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B51" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B52" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B53" t="s">
-        <v>51</v>
+        <v>79</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B54" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B55" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B56" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B57" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B58" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B59" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B60" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B61" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>94</v>
+        <v>121</v>
       </c>
       <c r="B62" t="s">
-        <v>95</v>
+        <v>122</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
@@ -1385,6 +1393,14 @@
         <v>119</v>
       </c>
       <c r="B77" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>120</v>
+      </c>
+      <c r="B78" t="s">
         <v>117</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add pyjosa module / add test cases / add cdot replace
</commit_message>
<xml_diff>
--- a/math_table.xlsx
+++ b/math_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Pycharm\Project\math2kor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daehan_kim\Desktop\hyperstudy\math2kor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C2468CF-1314-45DA-909F-77537F411E05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E8F92F-AFA4-42C6-90AE-688330A11E6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="166">
   <si>
     <t>a</t>
   </si>
@@ -560,7 +560,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>는 즉</t>
+    <t xml:space="preserve"> 따라서</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 따라서</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cdot</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 닷</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -929,10 +941,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B97"/>
+  <dimension ref="A1:B98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="D79" sqref="D79"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1474,7 +1486,7 @@
         <v>110</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>101</v>
+        <v>163</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
@@ -1519,31 +1531,31 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>114</v>
+        <v>164</v>
       </c>
       <c r="B73" t="s">
-        <v>115</v>
+        <v>165</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
+        <v>114</v>
+      </c>
+      <c r="B74" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
         <v>116</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B75" t="s">
         <v>117</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A75" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>119</v>
@@ -1551,23 +1563,23 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>124</v>
@@ -1575,145 +1587,153 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
-        <v>126</v>
+        <v>140</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>127</v>
+        <v>141</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>156</v>
+        <v>139</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
-        <v>142</v>
+        <v>155</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>143</v>
+        <v>156</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A98" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="B97" s="1" t="s">
+      <c r="B98" s="1" t="s">
         <v>160</v>
       </c>
     </row>

</xml_diff>